<commit_message>
navigation btns high contrast
</commit_message>
<xml_diff>
--- a/public/AddInfos/de/3.5.1.xlsx
+++ b/public/AddInfos/de/3.5.1.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
   <si>
     <t>Jahr</t>
   </si>
@@ -45,9 +45,6 @@
     <t>213 - 253</t>
   </si>
   <si>
-    <t>224 - 226</t>
-  </si>
-  <si>
     <t>223 - 265</t>
   </si>
   <si>
@@ -61,6 +58,15 @@
   </si>
   <si>
     <t>Deutsche Beobachtungsstelle für Drogen und Drogensucht (DBDD)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Anmerkung: </t>
+  </si>
+  <si>
+    <t>Geschätzte Werte</t>
+  </si>
+  <si>
+    <t>224 - 266</t>
   </si>
 </sst>
 </file>
@@ -172,11 +178,11 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -381,11 +387,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="185112064"/>
-        <c:axId val="40676736"/>
+        <c:axId val="182031872"/>
+        <c:axId val="41463168"/>
       </c:areaChart>
       <c:catAx>
-        <c:axId val="185112064"/>
+        <c:axId val="182031872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -415,7 +421,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="40676736"/>
+        <c:crossAx val="41463168"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -423,7 +429,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="40676736"/>
+        <c:axId val="41463168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -453,7 +459,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="185112064"/>
+        <c:crossAx val="182031872"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -883,7 +889,7 @@
   <dimension ref="A1:H41"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="K29" sqref="K29"/>
+      <selection activeCell="L20" sqref="L20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -914,23 +920,23 @@
     </row>
     <row r="3" spans="1:7" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="B3" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" s="9"/>
-      <c r="D3" s="9"/>
-      <c r="E3" s="9"/>
-      <c r="F3" s="9"/>
-      <c r="G3" s="9"/>
+        <v>12</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="10"/>
+      <c r="D3" s="10"/>
+      <c r="E3" s="10"/>
+      <c r="F3" s="10"/>
+      <c r="G3" s="10"/>
     </row>
     <row r="4" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
@@ -1008,7 +1014,7 @@
         <v>2015</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
@@ -1021,7 +1027,7 @@
         <v>2016</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
@@ -1031,7 +1037,7 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="4"/>
-      <c r="B12" s="10"/>
+      <c r="B12" s="9"/>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
@@ -1228,8 +1234,12 @@
       <c r="G33" s="1"/>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A34" s="1"/>
-      <c r="B34" s="1"/>
+      <c r="A34" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B34" s="7" t="s">
+        <v>15</v>
+      </c>
       <c r="C34" s="1"/>
       <c r="D34" s="1"/>
       <c r="E34" s="1"/>
@@ -1241,7 +1251,7 @@
         <v>1</v>
       </c>
       <c r="B35" s="7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C35" s="7"/>
       <c r="D35" s="1"/>
@@ -1324,7 +1334,7 @@
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:D7"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
updates and deletion of embedded feature related files
</commit_message>
<xml_diff>
--- a/public/AddInfos/de/3.5.1.xlsx
+++ b/public/AddInfos/de/3.5.1.xlsx
@@ -90,7 +90,7 @@
     <t>217 220 - 257 949</t>
   </si>
   <si>
-    <t>Schätzung des riskanten Konsums (auf Basis von Zugängen zu Behandlung) der Substanzen Opioide, Kokain und andere Stimulanzien im Alter von 15 bis unter 65 Jahren</t>
+    <t>Schätzung des riskanten Konsums (auf Basis von Zugängen zu Behandlung) der Substanzen Opioide, Kokain und anderer Stimulanzien im Alter von 15 bis unter 65 Jahren</t>
   </si>
 </sst>
 </file>
@@ -273,7 +273,7 @@
               <a:rPr lang="de-DE" sz="1400" b="1" i="0" baseline="0">
                 <a:effectLst/>
               </a:rPr>
-              <a:t>Schätzung des riskanten Konsums (auf Basis von Zugängen zu Behandlung) der Substanzen Opioide, Kokain und andere Stimulanzien im Alter von 15 bis unter 65 Jahren</a:t>
+              <a:t>Schätzung des riskanten Konsums (auf Basis von Zugängen zu Behandlung) der Substanzen Opioide, Kokain und anderer Stimulanzien im Alter von 15 bis unter 65 Jahren</a:t>
             </a:r>
             <a:endParaRPr lang="de-DE" sz="1100">
               <a:effectLst/>
@@ -281,6 +281,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -445,11 +446,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="182359552"/>
-        <c:axId val="59157888"/>
+        <c:axId val="177116672"/>
+        <c:axId val="41594240"/>
       </c:areaChart>
       <c:catAx>
-        <c:axId val="182359552"/>
+        <c:axId val="177116672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -472,13 +473,14 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="59157888"/>
+        <c:crossAx val="41594240"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -486,7 +488,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="59157888"/>
+        <c:axId val="41594240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -509,13 +511,14 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="182359552"/>
+        <c:crossAx val="177116672"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -557,7 +560,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="de-DE" sz="1400"/>
-              <a:t>Schätzung des riskanten Konsums (auf Basis von Zugängen zu Behandlung) der Substanzen Opioide, Kokain und andere Stimulanzien im Alter von 15 bis unter 65 Jahren</a:t>
+              <a:t>Schätzung des riskanten Konsums (auf Basis von Zugängen zu Behandlung) der Substanzen Opioide, Kokain und anderer Stimulanzien im Alter von 15 bis unter 65 Jahren</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -727,11 +730,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="176022016"/>
-        <c:axId val="59160768"/>
+        <c:axId val="158196224"/>
+        <c:axId val="41597120"/>
       </c:areaChart>
       <c:catAx>
-        <c:axId val="176022016"/>
+        <c:axId val="158196224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -761,7 +764,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="59160768"/>
+        <c:crossAx val="41597120"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -769,7 +772,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="59160768"/>
+        <c:axId val="41597120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -799,7 +802,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="176022016"/>
+        <c:crossAx val="158196224"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1353,8 +1356,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H41"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3:G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1802,8 +1805,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:G3"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>